<commit_message>
commit on January 19
</commit_message>
<xml_diff>
--- a/bin/com/puma/config/PumaTest.xlsx
+++ b/bin/com/puma/config/PumaTest.xlsx
@@ -719,7 +719,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -743,6 +743,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1095,13 +1101,14 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="16" customWidth="1"/>
+    <col min="1" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="16" style="10" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
@@ -1116,7 +1123,7 @@
       <c r="B1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1148,7 +1155,7 @@
       <c r="B2" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="14">
         <v>9255482255</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1178,7 +1185,7 @@
       <c r="B3" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1208,7 +1215,7 @@
       <c r="B4" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1238,7 +1245,7 @@
       <c r="B5" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1268,7 +1275,7 @@
       <c r="B6" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1298,7 +1305,7 @@
       <c r="B7" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="14" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1328,7 +1335,7 @@
       <c r="B8" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="14" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1358,7 +1365,7 @@
       <c r="B9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="14" t="s">
         <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1388,7 +1395,7 @@
       <c r="B10" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="14" t="s">
         <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1418,7 +1425,7 @@
       <c r="B11" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="14" t="s">
         <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1448,7 +1455,7 @@
       <c r="B12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="14" t="s">
         <v>82</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -1478,7 +1485,7 @@
       <c r="B13" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="14" t="s">
         <v>82</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1508,7 +1515,7 @@
       <c r="B14" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="14" t="s">
         <v>97</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1538,7 +1545,7 @@
       <c r="B15" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="14" t="s">
         <v>97</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1568,7 +1575,7 @@
       <c r="B16" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="14" t="s">
         <v>97</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1598,7 +1605,7 @@
       <c r="B17" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="14" t="s">
         <v>97</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1628,7 +1635,7 @@
       <c r="B18" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1658,6 +1665,9 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
+  <ignoredErrors>
+    <ignoredError sqref="C6" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
commit on January 20th
</commit_message>
<xml_diff>
--- a/bin/com/puma/config/PumaTest.xlsx
+++ b/bin/com/puma/config/PumaTest.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="40" windowWidth="31740" windowHeight="16700"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28440" windowHeight="15620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="Payment" sheetId="2" r:id="rId2"/>
+    <sheet name="5countries" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="182">
   <si>
     <t>FNAME</t>
   </si>
   <si>
+    <t xml:space="preserve"> LNAME</t>
+  </si>
+  <si>
     <t>PHONE</t>
   </si>
   <si>
@@ -52,6 +55,12 @@
     <t>fnameBrussel</t>
   </si>
   <si>
+    <t>regLname</t>
+  </si>
+  <si>
+    <t>9255431122</t>
+  </si>
+  <si>
     <t>test@yahoo.com</t>
   </si>
   <si>
@@ -415,159 +424,155 @@
     <t>Sweden</t>
   </si>
   <si>
-    <t>lnameBrussel</t>
-  </si>
-  <si>
-    <t>lnamePrague</t>
-  </si>
-  <si>
-    <t>lnameSCopenhagen</t>
-  </si>
-  <si>
-    <t>lnameTalinn</t>
-  </si>
-  <si>
-    <t>Barsa</t>
-  </si>
-  <si>
-    <t>lnAthens</t>
-  </si>
-  <si>
-    <t>lneMilan</t>
-  </si>
-  <si>
-    <t>LNAME</t>
-  </si>
-  <si>
-    <t>CREDIT_CARD_TYPE</t>
-  </si>
-  <si>
-    <t>SECURITY_CODE</t>
-  </si>
-  <si>
-    <t>EXP_MONTH</t>
-  </si>
-  <si>
-    <t>EXP_YEAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  verified_master 
-</t>
-  </si>
-  <si>
-    <t>950000000000000001</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  master_nosecurecode 
-</t>
-  </si>
-  <si>
-    <t>9500000000000002</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  verified_visa 
-</t>
-  </si>
-  <si>
-    <t>9400000000000003</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  visa_nosecurecode  
-</t>
-  </si>
-  <si>
-    <t>9400000000000004</t>
-  </si>
-  <si>
-    <t>033</t>
-  </si>
-  <si>
-    <t>321</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  verified_maestro 
-</t>
-  </si>
-  <si>
-    <t>9600000000000005</t>
-  </si>
-  <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  amex_nosecurecode 
-</t>
-  </si>
-  <si>
-    <t>9100000000000006</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  discover_nosecurecode 
-</t>
-  </si>
-  <si>
-    <t>9090000000000011</t>
-  </si>
-  <si>
-    <t>345</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>Iness</t>
-  </si>
-  <si>
-    <t>QA</t>
-  </si>
-  <si>
-    <t>ines'ss</t>
-  </si>
-  <si>
-    <t>ines</t>
-  </si>
-  <si>
-    <t>s'QA</t>
-  </si>
-  <si>
-    <t>qa</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>lastName2</t>
-  </si>
-  <si>
-    <t>lastName5</t>
-  </si>
-  <si>
-    <t>CARD_NUMBER</t>
+    <t>fnameRegSwitzerland</t>
+  </si>
+  <si>
+    <t>0871-423-4917</t>
+  </si>
+  <si>
+    <t>8153</t>
+  </si>
+  <si>
+    <t>Hofwisenstrasse</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Rümlang</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>fnameRegGermany</t>
+  </si>
+  <si>
+    <t>087423.4917</t>
+  </si>
+  <si>
+    <t>testGermany@hotmail.com</t>
+  </si>
+  <si>
+    <t>61169</t>
+  </si>
+  <si>
+    <t>Grüner Weg</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Friedberg</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>regPOBox</t>
+  </si>
+  <si>
+    <t>0874234917</t>
+  </si>
+  <si>
+    <t>80905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.O. Box </t>
+  </si>
+  <si>
+    <t>45 05 33</t>
+  </si>
+  <si>
+    <t>Munich</t>
+  </si>
+  <si>
+    <t>fnameRegUK</t>
+  </si>
+  <si>
+    <t>testUK@hotmail.com</t>
+  </si>
+  <si>
+    <t>W1D 3DH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richmond Mews </t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom </t>
+  </si>
+  <si>
+    <t>L75 1WX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Po Box </t>
+  </si>
+  <si>
+    <t>1970</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>SE3 0RL</t>
+  </si>
+  <si>
+    <t>Montpelier Row</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>fnameRegAustria</t>
+  </si>
+  <si>
+    <t>testAustria@hotmail.com</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fleischmarkt </t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Vienna</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>fnameRegFrance</t>
+  </si>
+  <si>
+    <t>testparis@hotmail.com</t>
+  </si>
+  <si>
+    <t>75008</t>
+  </si>
+  <si>
+    <t>Avenue George V</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>France</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -596,34 +601,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -635,20 +614,8 @@
         <fgColor indexed="31"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA2BD90"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFAECCBD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -671,55 +638,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -727,22 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -750,23 +660,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1099,16 +995,17 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="16" style="10" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="16" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
@@ -1120,554 +1017,548 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="14">
-        <v>9255482255</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="28">
       <c r="A4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10" outlineLevel="1">
       <c r="A5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10" outlineLevel="1">
       <c r="A6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10" outlineLevel="1">
       <c r="A7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="28">
       <c r="A8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>47</v>
+        <v>57</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="28" outlineLevel="1">
       <c r="A10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:10" outlineLevel="1">
       <c r="A11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>60</v>
+        <v>77</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28" outlineLevel="1">
       <c r="A12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:10" outlineLevel="1">
       <c r="A13" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>82</v>
+        <v>92</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28" outlineLevel="1">
       <c r="A14" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>97</v>
+        <v>107</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>97</v>
+        <v>113</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:10" outlineLevel="1">
       <c r="A17" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>97</v>
+        <v>119</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:10" outlineLevel="1">
       <c r="A18" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" outlineLevel="1">
-      <c r="B19" s="5"/>
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <ignoredErrors>
-    <ignoredError sqref="C6" numberStoredAsText="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1678,210 +1569,297 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView showFormulas="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.5" customWidth="1"/>
+    <col min="10" max="10" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" ht="18">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="J2" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="42">
-      <c r="A2" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" s="10">
-        <v>124</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="E2">
-        <v>2014</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="42">
-      <c r="A3" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="10">
-        <v>111</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="E3">
-        <v>2015</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28">
-      <c r="A4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4">
-        <v>2016</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="42">
-      <c r="A5" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5">
-        <v>2017</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="42">
-      <c r="A6" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6">
-        <v>2018</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="42">
-      <c r="A7" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="E7">
-        <v>2019</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="42">
-      <c r="A8" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="E8">
-        <v>2014</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15">
-      <c r="A14" s="12"/>
+      <c r="E9" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>181</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>